<commit_message>
Resultados 128 centroides, k-mean, Reagrupamiento, Mahalanobis
Pruebas con algoritmo principal utilizando mahalanobis con 128
centroides iniciales en k-means.
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>EXPERIMENTOS</t>
   </si>
@@ -47,59 +47,36 @@
     <t>Tolerancia</t>
   </si>
   <si>
-    <t>FCM</t>
-  </si>
-  <si>
     <t>Espacio de color</t>
   </si>
   <si>
-    <t>Images/35070</t>
-  </si>
-  <si>
-    <t>Results/insecto</t>
-  </si>
-  <si>
-    <t>Results/insecto2</t>
-  </si>
-  <si>
-    <t>Results/insecto3</t>
-  </si>
-  <si>
-    <t>Results/insecto4</t>
-  </si>
-  <si>
     <t>RGB</t>
   </si>
   <si>
-    <t>L a b</t>
-  </si>
-  <si>
-    <t>Results/insecto5</t>
-  </si>
-  <si>
-    <t>Results/insecto6</t>
-  </si>
-  <si>
-    <t>Results/insecto7</t>
-  </si>
-  <si>
-    <t>Results/insecto8</t>
+    <t>showimage</t>
+  </si>
+  <si>
+    <t>leucolinf</t>
+  </si>
+  <si>
+    <t>plain</t>
+  </si>
+  <si>
+    <t>metodo 1: k-means-Reagrupamiento-RGB-Mahalanobis</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>41004-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -129,10 +106,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -413,15 +390,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" customWidth="1"/>
+    <col min="1" max="1" width="51.28515625" customWidth="1"/>
     <col min="2" max="2" width="15.28515625" customWidth="1"/>
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
     <col min="4" max="4" width="19.85546875" customWidth="1"/>
@@ -431,25 +408,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -469,162 +446,225 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3">
+        <v>128</v>
+      </c>
+      <c r="F3">
+        <v>3.0482</v>
+      </c>
+      <c r="G3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="E3">
-        <v>4</v>
-      </c>
-      <c r="G3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F4">
+        <v>9.9550999999999998</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>1.9119999999999999</v>
+      </c>
+      <c r="G5">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4">
-        <v>8</v>
-      </c>
-      <c r="G4">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>16</v>
-      </c>
-      <c r="G5">
-        <v>16</v>
-      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
+      <c r="C6">
+        <v>60079</v>
+      </c>
+      <c r="F6">
+        <v>7.3141999999999996</v>
       </c>
       <c r="G6">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
+      <c r="C7">
+        <v>45096</v>
+      </c>
+      <c r="F7">
+        <v>2.2719999999999998</v>
       </c>
       <c r="G7">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" t="s">
-        <v>17</v>
-      </c>
-      <c r="E8">
-        <v>4</v>
+      <c r="C8">
+        <v>188091</v>
+      </c>
+      <c r="F8">
+        <v>5.8066000000000004</v>
       </c>
       <c r="G8">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" t="s">
-        <v>15</v>
-      </c>
       <c r="C9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="F9">
+        <v>3.2934000000000001</v>
       </c>
       <c r="G9">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10">
-        <v>16</v>
+      <c r="C10" s="1">
+        <v>253036</v>
+      </c>
+      <c r="F10">
+        <v>4.5782999999999996</v>
       </c>
       <c r="G10">
-        <v>16</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>42049</v>
+      </c>
+      <c r="F11">
+        <v>4.3924000000000003</v>
+      </c>
+      <c r="G11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>163014</v>
+      </c>
+      <c r="F13">
+        <v>3.8043</v>
+      </c>
+      <c r="G13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>124084</v>
+      </c>
+      <c r="F14">
+        <v>2.0809000000000002</v>
+      </c>
+      <c r="G14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>176035</v>
+      </c>
+      <c r="F15">
+        <v>3.0331000000000001</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <v>295087</v>
+      </c>
+      <c r="F16">
+        <v>4.1481000000000003</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <v>216066</v>
+      </c>
+      <c r="F17">
+        <v>4.5587999999999997</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18">
+        <v>3.5859999999999999</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <v>388016</v>
+      </c>
+      <c r="F19">
+        <v>4.1205999999999996</v>
+      </c>
+      <c r="G19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <v>385028</v>
+      </c>
+      <c r="F20">
+        <v>4.2629000000000001</v>
+      </c>
+      <c r="G20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <v>225017</v>
+      </c>
+      <c r="F21">
+        <v>3.8323</v>
+      </c>
+      <c r="G21">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <v>113044</v>
+      </c>
+      <c r="F22">
+        <v>6.3635999999999999</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pruebas con 64 centroides- dev
Pruebas con 64 centroides (metodo dos en Excel), algoritmo principal.
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="18">
   <si>
     <t>EXPERIMENTOS</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>41004-2</t>
+  </si>
+  <si>
+    <t>fabric</t>
+  </si>
+  <si>
+    <t>metodo 2: k-means-Reagrupamiento-RGB-Mahalanobis</t>
+  </si>
+  <si>
+    <t>12375764_10154354426419428_2121622626_o</t>
   </si>
 </sst>
 </file>
@@ -390,10 +399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -465,9 +474,18 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
       <c r="C4" t="s">
         <v>10</v>
       </c>
+      <c r="E4">
+        <v>128</v>
+      </c>
       <c r="F4">
         <v>9.9550999999999998</v>
       </c>
@@ -476,9 +494,18 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
       <c r="C5" t="s">
         <v>11</v>
       </c>
+      <c r="E5">
+        <v>128</v>
+      </c>
       <c r="F5">
         <v>1.9119999999999999</v>
       </c>
@@ -487,9 +514,18 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
       <c r="C6">
         <v>60079</v>
       </c>
+      <c r="E6">
+        <v>128</v>
+      </c>
       <c r="F6">
         <v>7.3141999999999996</v>
       </c>
@@ -498,9 +534,18 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
       <c r="C7">
         <v>45096</v>
       </c>
+      <c r="E7">
+        <v>128</v>
+      </c>
       <c r="F7">
         <v>2.2719999999999998</v>
       </c>
@@ -509,9 +554,18 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
       <c r="C8">
         <v>188091</v>
       </c>
+      <c r="E8">
+        <v>128</v>
+      </c>
       <c r="F8">
         <v>5.8066000000000004</v>
       </c>
@@ -520,9 +574,18 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
       <c r="C9" t="s">
         <v>13</v>
       </c>
+      <c r="E9">
+        <v>128</v>
+      </c>
       <c r="F9">
         <v>3.2934000000000001</v>
       </c>
@@ -531,9 +594,18 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" t="s">
+        <v>8</v>
+      </c>
       <c r="C10" s="1">
         <v>253036</v>
       </c>
+      <c r="E10">
+        <v>128</v>
+      </c>
       <c r="F10">
         <v>4.5782999999999996</v>
       </c>
@@ -542,9 +614,18 @@
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
       <c r="C11">
         <v>42049</v>
       </c>
+      <c r="E11">
+        <v>128</v>
+      </c>
       <c r="F11">
         <v>4.3924000000000003</v>
       </c>
@@ -553,14 +634,32 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
+      </c>
       <c r="D12">
         <v>12</v>
       </c>
+      <c r="E12">
+        <v>128</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
       <c r="C13">
         <v>163014</v>
       </c>
+      <c r="E13">
+        <v>128</v>
+      </c>
       <c r="F13">
         <v>3.8043</v>
       </c>
@@ -569,9 +668,18 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
       <c r="C14">
         <v>124084</v>
       </c>
+      <c r="E14">
+        <v>128</v>
+      </c>
       <c r="F14">
         <v>2.0809000000000002</v>
       </c>
@@ -580,9 +688,18 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>8</v>
+      </c>
       <c r="C15">
         <v>176035</v>
       </c>
+      <c r="E15">
+        <v>128</v>
+      </c>
       <c r="F15">
         <v>3.0331000000000001</v>
       </c>
@@ -591,9 +708,18 @@
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
+        <v>8</v>
+      </c>
       <c r="C16">
         <v>295087</v>
       </c>
+      <c r="E16">
+        <v>128</v>
+      </c>
       <c r="F16">
         <v>4.1481000000000003</v>
       </c>
@@ -601,10 +727,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
       <c r="C17">
         <v>216066</v>
       </c>
+      <c r="E17">
+        <v>128</v>
+      </c>
       <c r="F17">
         <v>4.5587999999999997</v>
       </c>
@@ -612,10 +747,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
       <c r="C18" t="s">
         <v>14</v>
       </c>
+      <c r="E18">
+        <v>128</v>
+      </c>
       <c r="F18">
         <v>3.5859999999999999</v>
       </c>
@@ -623,10 +767,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>8</v>
+      </c>
       <c r="C19">
         <v>388016</v>
       </c>
+      <c r="E19">
+        <v>128</v>
+      </c>
       <c r="F19">
         <v>4.1205999999999996</v>
       </c>
@@ -634,10 +787,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
       <c r="C20">
         <v>385028</v>
       </c>
+      <c r="E20">
+        <v>128</v>
+      </c>
       <c r="F20">
         <v>4.2629000000000001</v>
       </c>
@@ -645,10 +807,19 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" t="s">
+        <v>8</v>
+      </c>
       <c r="C21">
         <v>225017</v>
       </c>
+      <c r="E21">
+        <v>128</v>
+      </c>
       <c r="F21">
         <v>3.8323</v>
       </c>
@@ -656,15 +827,110 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
       <c r="C22">
         <v>113044</v>
       </c>
+      <c r="E22">
+        <v>128</v>
+      </c>
       <c r="F22">
         <v>6.3635999999999999</v>
       </c>
       <c r="G22">
         <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>64</v>
+      </c>
+      <c r="F23">
+        <v>2.1093999999999999</v>
+      </c>
+      <c r="G23">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24">
+        <v>2.8155000000000001</v>
+      </c>
+      <c r="G24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <v>113044</v>
+      </c>
+      <c r="F25">
+        <v>3.3246000000000002</v>
+      </c>
+      <c r="G25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <v>225017</v>
+      </c>
+      <c r="F26">
+        <v>2.0082</v>
+      </c>
+      <c r="G26">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>385028</v>
+      </c>
+      <c r="F27">
+        <v>2.2035999999999998</v>
+      </c>
+      <c r="G27">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <v>388016</v>
+      </c>
+      <c r="F28">
+        <v>2.3083999999999998</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29">
+        <v>1.8198000000000001</v>
+      </c>
+      <c r="G29">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pruebas con 64 centroides
resultados con 64 centroides iniciales
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="21">
   <si>
     <t>EXPERIMENTOS</t>
   </si>
@@ -78,6 +78,15 @@
   </si>
   <si>
     <t>12375764_10154354426419428_2121622626_o</t>
+  </si>
+  <si>
+    <t>Plain</t>
+  </si>
+  <si>
+    <t>linfocitos1</t>
+  </si>
+  <si>
+    <t>10472953_992127864183797_1990666493_n</t>
   </si>
 </sst>
 </file>
@@ -399,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,6 +880,9 @@
       <c r="C24" t="s">
         <v>17</v>
       </c>
+      <c r="E24">
+        <v>64</v>
+      </c>
       <c r="F24">
         <v>2.8155000000000001</v>
       </c>
@@ -882,6 +894,9 @@
       <c r="C25">
         <v>113044</v>
       </c>
+      <c r="E25">
+        <v>64</v>
+      </c>
       <c r="F25">
         <v>3.3246000000000002</v>
       </c>
@@ -893,6 +908,9 @@
       <c r="C26">
         <v>225017</v>
       </c>
+      <c r="E26">
+        <v>64</v>
+      </c>
       <c r="F26">
         <v>2.0082</v>
       </c>
@@ -904,6 +922,9 @@
       <c r="C27">
         <v>385028</v>
       </c>
+      <c r="E27">
+        <v>64</v>
+      </c>
       <c r="F27">
         <v>2.2035999999999998</v>
       </c>
@@ -915,6 +936,9 @@
       <c r="C28">
         <v>388016</v>
       </c>
+      <c r="E28">
+        <v>64</v>
+      </c>
       <c r="F28">
         <v>2.3083999999999998</v>
       </c>
@@ -926,11 +950,280 @@
       <c r="C29" t="s">
         <v>14</v>
       </c>
+      <c r="E29">
+        <v>64</v>
+      </c>
       <c r="F29">
         <v>1.8198000000000001</v>
       </c>
       <c r="G29">
         <v>6</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <v>216066</v>
+      </c>
+      <c r="E30">
+        <v>64</v>
+      </c>
+      <c r="F30">
+        <v>3.0548000000000002</v>
+      </c>
+      <c r="G30">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <v>295087</v>
+      </c>
+      <c r="E31">
+        <v>64</v>
+      </c>
+      <c r="F31">
+        <v>2.0613999999999999</v>
+      </c>
+      <c r="G31">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <v>176035</v>
+      </c>
+      <c r="E32">
+        <v>64</v>
+      </c>
+      <c r="F32">
+        <v>1.6104000000000001</v>
+      </c>
+      <c r="G32">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <v>296059</v>
+      </c>
+      <c r="E33">
+        <v>64</v>
+      </c>
+      <c r="F33">
+        <v>2.7111000000000001</v>
+      </c>
+      <c r="G33">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <v>124084</v>
+      </c>
+      <c r="E34">
+        <v>64</v>
+      </c>
+      <c r="F34">
+        <v>1.0268999999999999</v>
+      </c>
+      <c r="G34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <v>163014</v>
+      </c>
+      <c r="E35">
+        <v>64</v>
+      </c>
+      <c r="F35">
+        <v>2.3742000000000001</v>
+      </c>
+      <c r="G35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <v>35070</v>
+      </c>
+      <c r="E36">
+        <v>64</v>
+      </c>
+      <c r="F36">
+        <v>2.3170000000000002</v>
+      </c>
+      <c r="G36">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <v>42049</v>
+      </c>
+      <c r="E37">
+        <v>64</v>
+      </c>
+      <c r="F37">
+        <v>2.2507999999999999</v>
+      </c>
+      <c r="G37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <v>253036</v>
+      </c>
+      <c r="E38">
+        <v>64</v>
+      </c>
+      <c r="F38">
+        <v>2.5701999999999998</v>
+      </c>
+      <c r="G38">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39">
+        <v>64</v>
+      </c>
+      <c r="F39">
+        <v>1.7512000000000001</v>
+      </c>
+      <c r="G39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <v>188091</v>
+      </c>
+      <c r="E40">
+        <v>64</v>
+      </c>
+      <c r="F40">
+        <v>2.6861000000000002</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <v>45096</v>
+      </c>
+      <c r="E41">
+        <v>64</v>
+      </c>
+      <c r="F41">
+        <v>1.0215000000000001</v>
+      </c>
+      <c r="G41">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <v>60079</v>
+      </c>
+      <c r="E42">
+        <v>64</v>
+      </c>
+      <c r="F42">
+        <v>4.1104000000000003</v>
+      </c>
+      <c r="G42">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E43">
+        <v>64</v>
+      </c>
+      <c r="F43">
+        <v>0.82157999999999998</v>
+      </c>
+      <c r="G43">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E44">
+        <v>64</v>
+      </c>
+      <c r="F44">
+        <v>1.2588999999999999</v>
+      </c>
+      <c r="G44">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C45" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45">
+        <v>64</v>
+      </c>
+      <c r="F45">
+        <v>4.5297999999999998</v>
+      </c>
+      <c r="G45">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <v>135069</v>
+      </c>
+      <c r="E46">
+        <v>64</v>
+      </c>
+      <c r="F46">
+        <v>2.6396000000000002</v>
+      </c>
+      <c r="G46">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
+        <v>19</v>
+      </c>
+      <c r="E47">
+        <v>64</v>
+      </c>
+      <c r="F47">
+        <v>5.4508999999999999</v>
+      </c>
+      <c r="G47">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
+        <v>20</v>
+      </c>
+      <c r="E48">
+        <v>64</v>
+      </c>
+      <c r="F48">
+        <v>1.2169000000000001</v>
+      </c>
+      <c r="G48">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Pruebas con 32 centroides iniciales
otras pruebas con tercer método
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="22">
   <si>
     <t>EXPERIMENTOS</t>
   </si>
@@ -411,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B46" workbookViewId="0">
-      <selection activeCell="G59" sqref="G59"/>
+    <sheetView tabSelected="1" topLeftCell="B58" workbookViewId="0">
+      <selection activeCell="F69" sqref="F69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1465,6 +1465,149 @@
         <v>7</v>
       </c>
     </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <v>45096</v>
+      </c>
+      <c r="F56">
+        <v>53.078000000000003</v>
+      </c>
+      <c r="G56">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <v>188091</v>
+      </c>
+      <c r="F57">
+        <v>24.049600000000002</v>
+      </c>
+      <c r="G57">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C58" t="s">
+        <v>13</v>
+      </c>
+      <c r="F58">
+        <v>38.966500000000003</v>
+      </c>
+      <c r="G58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <v>253036</v>
+      </c>
+      <c r="F59">
+        <v>28.33</v>
+      </c>
+      <c r="G59">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <v>42049</v>
+      </c>
+      <c r="F60">
+        <v>24.692299999999999</v>
+      </c>
+      <c r="G60">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <v>35070</v>
+      </c>
+      <c r="F61">
+        <v>17.706499999999998</v>
+      </c>
+      <c r="G61">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <v>163014</v>
+      </c>
+      <c r="F62">
+        <v>18.2836</v>
+      </c>
+      <c r="G62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <v>124084</v>
+      </c>
+      <c r="F63">
+        <v>51.0747</v>
+      </c>
+      <c r="G63">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <v>296059</v>
+      </c>
+      <c r="F64">
+        <v>19.521699999999999</v>
+      </c>
+      <c r="G64">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <v>176035</v>
+      </c>
+      <c r="F65">
+        <v>39.887500000000003</v>
+      </c>
+      <c r="G65">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="66" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <v>295087</v>
+      </c>
+      <c r="F66">
+        <v>20.520399999999999</v>
+      </c>
+      <c r="G66">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="67" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <v>216066</v>
+      </c>
+      <c r="F67">
+        <v>16.633900000000001</v>
+      </c>
+      <c r="G67">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="68" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>14</v>
+      </c>
+      <c r="F68">
+        <v>36.705500000000001</v>
+      </c>
+      <c r="G68">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>

</xml_diff>

<commit_message>
Pruebas con 64 centroiedes
Pruebas con 64 centroides método 4
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="22">
   <si>
     <t>EXPERIMENTOS</t>
   </si>
@@ -411,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J78"/>
+  <dimension ref="A1:J88"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B73" workbookViewId="0">
-      <selection activeCell="E84" sqref="E84"/>
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1718,6 +1718,116 @@
         <v>4</v>
       </c>
     </row>
+    <row r="79" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79">
+        <v>28.3733</v>
+      </c>
+      <c r="G79">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="80" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <v>60079</v>
+      </c>
+      <c r="F80">
+        <v>6.3574999999999999</v>
+      </c>
+      <c r="G80">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="81" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <v>45096</v>
+      </c>
+      <c r="F81">
+        <v>27.905799999999999</v>
+      </c>
+      <c r="G81">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="82" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <v>188091</v>
+      </c>
+      <c r="F82">
+        <v>10.9636</v>
+      </c>
+      <c r="G82">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="83" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>13</v>
+      </c>
+      <c r="F83">
+        <v>20.583500000000001</v>
+      </c>
+      <c r="G83">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="84" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <v>253036</v>
+      </c>
+      <c r="F84">
+        <v>13.8782</v>
+      </c>
+      <c r="G84">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <v>42049</v>
+      </c>
+      <c r="F85">
+        <v>13.3101</v>
+      </c>
+      <c r="G85">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="86" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <v>35070</v>
+      </c>
+      <c r="F86">
+        <v>9.7677999999999994</v>
+      </c>
+      <c r="G86">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C87">
+        <v>163014</v>
+      </c>
+      <c r="F87">
+        <v>10.9528</v>
+      </c>
+      <c r="G87">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="88" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C88">
+        <v>124084</v>
+      </c>
+      <c r="F88">
+        <v>26.652000000000001</v>
+      </c>
+      <c r="G88">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>

</xml_diff>

<commit_message>
Pruebas con rgb y mahalanobis - kmeans
Se establecio un rango de tolerancia para el agrupamiento utilizando
mahalanobis y RGB
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -303,6 +303,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -311,11 +316,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -604,8 +604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A119" workbookViewId="0">
-      <selection activeCell="C133" sqref="C133"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F53" sqref="F53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,18 +620,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="12"/>
-      <c r="J1" s="13"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:10" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9" t="s">
@@ -867,7 +867,7 @@
       <c r="F13">
         <v>3.8043</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="13">
         <v>4</v>
       </c>
     </row>
@@ -1061,7 +1061,7 @@
       <c r="C23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="14">
+      <c r="E23" s="11">
         <v>64</v>
       </c>
       <c r="F23">
@@ -1081,7 +1081,7 @@
       <c r="C24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="14">
+      <c r="E24" s="11">
         <v>64</v>
       </c>
       <c r="F24">
@@ -1101,7 +1101,7 @@
       <c r="C25" s="3">
         <v>113044</v>
       </c>
-      <c r="E25" s="14">
+      <c r="E25" s="11">
         <v>64</v>
       </c>
       <c r="F25">
@@ -1121,7 +1121,7 @@
       <c r="C26" s="3">
         <v>225017</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="11">
         <v>64</v>
       </c>
       <c r="F26">
@@ -1141,7 +1141,7 @@
       <c r="C27" s="3">
         <v>385028</v>
       </c>
-      <c r="E27" s="14">
+      <c r="E27" s="11">
         <v>64</v>
       </c>
       <c r="F27">
@@ -1161,7 +1161,7 @@
       <c r="C28" s="3">
         <v>388016</v>
       </c>
-      <c r="E28" s="14">
+      <c r="E28" s="11">
         <v>64</v>
       </c>
       <c r="F28">
@@ -1181,7 +1181,7 @@
       <c r="C29" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E29" s="14">
+      <c r="E29" s="11">
         <v>64</v>
       </c>
       <c r="F29">
@@ -1201,7 +1201,7 @@
       <c r="C30" s="3">
         <v>216066</v>
       </c>
-      <c r="E30" s="14">
+      <c r="E30" s="11">
         <v>64</v>
       </c>
       <c r="F30">
@@ -1221,7 +1221,7 @@
       <c r="C31" s="3">
         <v>295087</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="11">
         <v>64</v>
       </c>
       <c r="F31">
@@ -1241,7 +1241,7 @@
       <c r="C32" s="3">
         <v>176035</v>
       </c>
-      <c r="E32" s="14">
+      <c r="E32" s="11">
         <v>64</v>
       </c>
       <c r="F32">
@@ -1261,7 +1261,7 @@
       <c r="C33" s="3">
         <v>296059</v>
       </c>
-      <c r="E33" s="14">
+      <c r="E33" s="11">
         <v>64</v>
       </c>
       <c r="F33">
@@ -1281,7 +1281,7 @@
       <c r="C34" s="3">
         <v>124084</v>
       </c>
-      <c r="E34" s="14">
+      <c r="E34" s="11">
         <v>64</v>
       </c>
       <c r="F34">
@@ -1301,7 +1301,7 @@
       <c r="C35" s="3">
         <v>163014</v>
       </c>
-      <c r="E35" s="14">
+      <c r="E35" s="11">
         <v>64</v>
       </c>
       <c r="F35">
@@ -1321,7 +1321,7 @@
       <c r="C36" s="3">
         <v>35070</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="11">
         <v>64</v>
       </c>
       <c r="F36">
@@ -1341,7 +1341,7 @@
       <c r="C37" s="3">
         <v>42049</v>
       </c>
-      <c r="E37" s="14">
+      <c r="E37" s="11">
         <v>64</v>
       </c>
       <c r="F37">
@@ -1361,7 +1361,7 @@
       <c r="C38" s="3">
         <v>253036</v>
       </c>
-      <c r="E38" s="14">
+      <c r="E38" s="11">
         <v>64</v>
       </c>
       <c r="F38">
@@ -1381,7 +1381,7 @@
       <c r="C39" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E39" s="14">
+      <c r="E39" s="11">
         <v>64</v>
       </c>
       <c r="F39">
@@ -1401,7 +1401,7 @@
       <c r="C40" s="3">
         <v>188091</v>
       </c>
-      <c r="E40" s="14">
+      <c r="E40" s="11">
         <v>64</v>
       </c>
       <c r="F40">
@@ -1421,7 +1421,7 @@
       <c r="C41" s="3">
         <v>45096</v>
       </c>
-      <c r="E41" s="14">
+      <c r="E41" s="11">
         <v>64</v>
       </c>
       <c r="F41">
@@ -1441,7 +1441,7 @@
       <c r="C42" s="3">
         <v>60079</v>
       </c>
-      <c r="E42" s="14">
+      <c r="E42" s="11">
         <v>64</v>
       </c>
       <c r="F42">
@@ -1461,7 +1461,7 @@
       <c r="C43" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E43" s="14">
+      <c r="E43" s="11">
         <v>64</v>
       </c>
       <c r="F43">
@@ -1481,7 +1481,7 @@
       <c r="C44" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E44" s="14">
+      <c r="E44" s="11">
         <v>64</v>
       </c>
       <c r="F44">
@@ -1501,7 +1501,7 @@
       <c r="C45" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E45" s="14">
+      <c r="E45" s="11">
         <v>64</v>
       </c>
       <c r="F45">
@@ -1521,7 +1521,7 @@
       <c r="C46" s="3">
         <v>135069</v>
       </c>
-      <c r="E46" s="14">
+      <c r="E46" s="11">
         <v>64</v>
       </c>
       <c r="F46">
@@ -1541,7 +1541,7 @@
       <c r="C47" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E47" s="14">
+      <c r="E47" s="11">
         <v>64</v>
       </c>
       <c r="F47">
@@ -1561,7 +1561,7 @@
       <c r="C48" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E48" s="14">
+      <c r="E48" s="11">
         <v>64</v>
       </c>
       <c r="F48">
@@ -1581,7 +1581,7 @@
       <c r="C49" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E49" s="15">
+      <c r="E49" s="12">
         <v>32</v>
       </c>
       <c r="F49">
@@ -1601,7 +1601,7 @@
       <c r="C50" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E50" s="15">
+      <c r="E50" s="12">
         <v>32</v>
       </c>
       <c r="F50">
@@ -1621,7 +1621,7 @@
       <c r="C51" s="3">
         <v>135069</v>
       </c>
-      <c r="E51" s="15">
+      <c r="E51" s="12">
         <v>32</v>
       </c>
       <c r="F51">
@@ -1641,7 +1641,7 @@
       <c r="C52" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E52" s="15">
+      <c r="E52" s="12">
         <v>32</v>
       </c>
       <c r="F52">
@@ -1661,7 +1661,7 @@
       <c r="C53" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E53" s="15">
+      <c r="E53" s="12">
         <v>32</v>
       </c>
       <c r="F53">
@@ -1681,7 +1681,7 @@
       <c r="C54" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E54" s="15">
+      <c r="E54" s="12">
         <v>32</v>
       </c>
       <c r="F54">
@@ -1701,7 +1701,7 @@
       <c r="C55" s="3">
         <v>60079</v>
       </c>
-      <c r="E55" s="15">
+      <c r="E55" s="12">
         <v>32</v>
       </c>
       <c r="F55">
@@ -1721,7 +1721,7 @@
       <c r="C56" s="3">
         <v>45096</v>
       </c>
-      <c r="E56" s="15">
+      <c r="E56" s="12">
         <v>32</v>
       </c>
       <c r="F56">
@@ -1741,7 +1741,7 @@
       <c r="C57" s="3">
         <v>188091</v>
       </c>
-      <c r="E57" s="15">
+      <c r="E57" s="12">
         <v>32</v>
       </c>
       <c r="F57">
@@ -1761,7 +1761,7 @@
       <c r="C58" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E58" s="15">
+      <c r="E58" s="12">
         <v>32</v>
       </c>
       <c r="F58">
@@ -1781,7 +1781,7 @@
       <c r="C59" s="3">
         <v>253036</v>
       </c>
-      <c r="E59" s="15">
+      <c r="E59" s="12">
         <v>32</v>
       </c>
       <c r="F59">
@@ -1801,7 +1801,7 @@
       <c r="C60" s="3">
         <v>42049</v>
       </c>
-      <c r="E60" s="15">
+      <c r="E60" s="12">
         <v>32</v>
       </c>
       <c r="F60">
@@ -1821,7 +1821,7 @@
       <c r="C61" s="3">
         <v>35070</v>
       </c>
-      <c r="E61" s="15">
+      <c r="E61" s="12">
         <v>32</v>
       </c>
       <c r="F61">
@@ -1841,7 +1841,7 @@
       <c r="C62" s="3">
         <v>163014</v>
       </c>
-      <c r="E62" s="15">
+      <c r="E62" s="12">
         <v>32</v>
       </c>
       <c r="F62">
@@ -1861,7 +1861,7 @@
       <c r="C63" s="3">
         <v>124084</v>
       </c>
-      <c r="E63" s="15">
+      <c r="E63" s="12">
         <v>32</v>
       </c>
       <c r="F63">
@@ -1881,7 +1881,7 @@
       <c r="C64" s="3">
         <v>296059</v>
       </c>
-      <c r="E64" s="15">
+      <c r="E64" s="12">
         <v>32</v>
       </c>
       <c r="F64">
@@ -1901,7 +1901,7 @@
       <c r="C65" s="3">
         <v>176035</v>
       </c>
-      <c r="E65" s="15">
+      <c r="E65" s="12">
         <v>32</v>
       </c>
       <c r="F65">
@@ -1921,7 +1921,7 @@
       <c r="C66" s="3">
         <v>295087</v>
       </c>
-      <c r="E66" s="15">
+      <c r="E66" s="12">
         <v>32</v>
       </c>
       <c r="F66">
@@ -1941,7 +1941,7 @@
       <c r="C67" s="3">
         <v>216066</v>
       </c>
-      <c r="E67" s="15">
+      <c r="E67" s="12">
         <v>32</v>
       </c>
       <c r="F67">
@@ -1961,7 +1961,7 @@
       <c r="C68" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E68" s="15">
+      <c r="E68" s="12">
         <v>32</v>
       </c>
       <c r="F68">
@@ -1981,7 +1981,7 @@
       <c r="C69" s="3">
         <v>388016</v>
       </c>
-      <c r="E69" s="15">
+      <c r="E69" s="12">
         <v>32</v>
       </c>
       <c r="F69">
@@ -2001,7 +2001,7 @@
       <c r="C70" s="3">
         <v>225017</v>
       </c>
-      <c r="E70" s="15">
+      <c r="E70" s="12">
         <v>32</v>
       </c>
       <c r="F70">
@@ -2021,7 +2021,7 @@
       <c r="C71" s="3">
         <v>113044</v>
       </c>
-      <c r="E71" s="15">
+      <c r="E71" s="12">
         <v>32</v>
       </c>
       <c r="F71">
@@ -2041,7 +2041,7 @@
       <c r="C72" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E72" s="15">
+      <c r="E72" s="12">
         <v>32</v>
       </c>
       <c r="F72">
@@ -2061,7 +2061,7 @@
       <c r="C73" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E73" s="15">
+      <c r="E73" s="12">
         <v>32</v>
       </c>
       <c r="F73">
@@ -2081,7 +2081,7 @@
       <c r="C74" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E74" s="15">
+      <c r="E74" s="12">
         <v>32</v>
       </c>
       <c r="F74">
@@ -2101,7 +2101,7 @@
       <c r="C75" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E75" s="15">
+      <c r="E75" s="12">
         <v>32</v>
       </c>
       <c r="F75">
@@ -2121,7 +2121,7 @@
       <c r="C76" s="3">
         <v>135069</v>
       </c>
-      <c r="E76" s="15">
+      <c r="E76" s="12">
         <v>32</v>
       </c>
       <c r="F76">
@@ -2141,7 +2141,7 @@
       <c r="C77" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E77" s="15">
+      <c r="E77" s="12">
         <v>32</v>
       </c>
       <c r="F77">
@@ -2161,7 +2161,7 @@
       <c r="C78" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E78" s="15">
+      <c r="E78" s="12">
         <v>32</v>
       </c>
       <c r="F78">
@@ -2181,7 +2181,7 @@
       <c r="C79" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E79" s="15">
+      <c r="E79" s="12">
         <v>32</v>
       </c>
       <c r="F79">
@@ -2201,7 +2201,7 @@
       <c r="C80" s="3">
         <v>60079</v>
       </c>
-      <c r="E80" s="15">
+      <c r="E80" s="12">
         <v>32</v>
       </c>
       <c r="F80">
@@ -2221,7 +2221,7 @@
       <c r="C81" s="3">
         <v>45096</v>
       </c>
-      <c r="E81" s="15">
+      <c r="E81" s="12">
         <v>32</v>
       </c>
       <c r="F81">
@@ -2241,7 +2241,7 @@
       <c r="C82" s="3">
         <v>188091</v>
       </c>
-      <c r="E82" s="15">
+      <c r="E82" s="12">
         <v>32</v>
       </c>
       <c r="F82">
@@ -2261,7 +2261,7 @@
       <c r="C83" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="E83" s="15">
+      <c r="E83" s="12">
         <v>32</v>
       </c>
       <c r="F83">
@@ -2281,7 +2281,7 @@
       <c r="C84" s="3">
         <v>253036</v>
       </c>
-      <c r="E84" s="15">
+      <c r="E84" s="12">
         <v>32</v>
       </c>
       <c r="F84">
@@ -2301,7 +2301,7 @@
       <c r="C85" s="3">
         <v>42049</v>
       </c>
-      <c r="E85" s="15">
+      <c r="E85" s="12">
         <v>32</v>
       </c>
       <c r="F85">
@@ -2321,7 +2321,7 @@
       <c r="C86" s="3">
         <v>35070</v>
       </c>
-      <c r="E86" s="15">
+      <c r="E86" s="12">
         <v>32</v>
       </c>
       <c r="F86">
@@ -2341,7 +2341,7 @@
       <c r="C87" s="3">
         <v>163014</v>
       </c>
-      <c r="E87" s="15">
+      <c r="E87" s="12">
         <v>32</v>
       </c>
       <c r="F87">
@@ -2361,7 +2361,7 @@
       <c r="C88" s="3">
         <v>124084</v>
       </c>
-      <c r="E88" s="15">
+      <c r="E88" s="12">
         <v>32</v>
       </c>
       <c r="F88">
@@ -2381,7 +2381,7 @@
       <c r="C89" s="3">
         <v>296059</v>
       </c>
-      <c r="E89" s="15">
+      <c r="E89" s="12">
         <v>32</v>
       </c>
       <c r="F89">
@@ -2401,7 +2401,7 @@
       <c r="C90" s="3">
         <v>176035</v>
       </c>
-      <c r="E90" s="15">
+      <c r="E90" s="12">
         <v>32</v>
       </c>
       <c r="F90">
@@ -2421,7 +2421,7 @@
       <c r="C91" s="3">
         <v>295087</v>
       </c>
-      <c r="E91" s="15">
+      <c r="E91" s="12">
         <v>32</v>
       </c>
       <c r="F91">
@@ -2441,7 +2441,7 @@
       <c r="C92" s="3">
         <v>216066</v>
       </c>
-      <c r="E92" s="15">
+      <c r="E92" s="12">
         <v>32</v>
       </c>
       <c r="F92">
@@ -2461,7 +2461,7 @@
       <c r="C93" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E93" s="15">
+      <c r="E93" s="12">
         <v>32</v>
       </c>
       <c r="F93">
@@ -2481,7 +2481,7 @@
       <c r="C94" s="3">
         <v>388016</v>
       </c>
-      <c r="E94" s="15">
+      <c r="E94" s="12">
         <v>32</v>
       </c>
       <c r="F94">
@@ -2501,7 +2501,7 @@
       <c r="C95" s="3">
         <v>385028</v>
       </c>
-      <c r="E95" s="15">
+      <c r="E95" s="12">
         <v>32</v>
       </c>
       <c r="F95">
@@ -2521,7 +2521,7 @@
       <c r="C96" s="3">
         <v>225017</v>
       </c>
-      <c r="E96" s="15">
+      <c r="E96" s="12">
         <v>32</v>
       </c>
       <c r="F96">
@@ -2541,7 +2541,7 @@
       <c r="C97" s="3">
         <v>113044</v>
       </c>
-      <c r="E97" s="15">
+      <c r="E97" s="12">
         <v>32</v>
       </c>
       <c r="F97">
@@ -2561,7 +2561,7 @@
       <c r="C98" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E98" s="15">
+      <c r="E98" s="12">
         <v>32</v>
       </c>
       <c r="F98">
@@ -2581,7 +2581,7 @@
       <c r="C99" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E99" s="15">
+      <c r="E99" s="12">
         <v>32</v>
       </c>
       <c r="F99" s="1">
@@ -2604,7 +2604,7 @@
       <c r="D100" t="s">
         <v>22</v>
       </c>
-      <c r="E100" s="15">
+      <c r="E100" s="12">
         <v>32</v>
       </c>
       <c r="F100">
@@ -2624,7 +2624,7 @@
       <c r="C101" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E101" s="15">
+      <c r="E101" s="12">
         <v>32</v>
       </c>
       <c r="F101">
@@ -2644,7 +2644,7 @@
       <c r="C102" s="3">
         <v>135069</v>
       </c>
-      <c r="E102" s="15">
+      <c r="E102" s="12">
         <v>32</v>
       </c>
       <c r="F102">
@@ -2664,7 +2664,7 @@
       <c r="C103" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E103" s="15">
+      <c r="E103" s="12">
         <v>32</v>
       </c>
       <c r="F103">
@@ -2684,7 +2684,7 @@
       <c r="C104" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E104" s="15">
+      <c r="E104" s="12">
         <v>32</v>
       </c>
       <c r="F104">
@@ -2704,7 +2704,7 @@
       <c r="C105" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="E105" s="15">
+      <c r="E105" s="12">
         <v>32</v>
       </c>
       <c r="F105">
@@ -2724,7 +2724,7 @@
       <c r="C106" s="3">
         <v>60079</v>
       </c>
-      <c r="E106" s="15">
+      <c r="E106" s="12">
         <v>32</v>
       </c>
       <c r="F106">
@@ -2744,7 +2744,7 @@
       <c r="C107" s="3">
         <v>45096</v>
       </c>
-      <c r="E107" s="15">
+      <c r="E107" s="12">
         <v>32</v>
       </c>
       <c r="F107">
@@ -2764,7 +2764,7 @@
       <c r="C108" s="3">
         <v>253036</v>
       </c>
-      <c r="E108" s="15">
+      <c r="E108" s="12">
         <v>32</v>
       </c>
       <c r="F108">
@@ -2781,7 +2781,7 @@
       <c r="C109" s="3">
         <v>42049</v>
       </c>
-      <c r="E109" s="15">
+      <c r="E109" s="12">
         <v>32</v>
       </c>
       <c r="F109">
@@ -2798,7 +2798,7 @@
       <c r="C110" s="3">
         <v>35070</v>
       </c>
-      <c r="E110" s="15">
+      <c r="E110" s="12">
         <v>32</v>
       </c>
       <c r="F110">
@@ -2815,7 +2815,7 @@
       <c r="C111" s="3">
         <v>101087</v>
       </c>
-      <c r="E111" s="15">
+      <c r="E111" s="12">
         <v>32</v>
       </c>
       <c r="F111">
@@ -2832,7 +2832,7 @@
       <c r="C112" s="3">
         <v>163014</v>
       </c>
-      <c r="E112" s="15">
+      <c r="E112" s="12">
         <v>32</v>
       </c>
       <c r="F112">
@@ -2852,7 +2852,7 @@
       <c r="C113" s="3">
         <v>124084</v>
       </c>
-      <c r="E113" s="15">
+      <c r="E113" s="12">
         <v>32</v>
       </c>
       <c r="F113">
@@ -2872,7 +2872,7 @@
       <c r="C114" s="3">
         <v>296059</v>
       </c>
-      <c r="E114" s="15">
+      <c r="E114" s="12">
         <v>32</v>
       </c>
       <c r="F114">
@@ -2892,7 +2892,7 @@
       <c r="C115" s="3">
         <v>176035</v>
       </c>
-      <c r="E115" s="15">
+      <c r="E115" s="12">
         <v>32</v>
       </c>
       <c r="F115">
@@ -2912,7 +2912,7 @@
       <c r="C116" s="3">
         <v>295087</v>
       </c>
-      <c r="E116" s="15">
+      <c r="E116" s="12">
         <v>32</v>
       </c>
       <c r="F116">
@@ -2932,7 +2932,7 @@
       <c r="C117" s="3">
         <v>216066</v>
       </c>
-      <c r="E117" s="15">
+      <c r="E117" s="12">
         <v>32</v>
       </c>
       <c r="F117">
@@ -2952,7 +2952,7 @@
       <c r="C118" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="E118" s="15">
+      <c r="E118" s="12">
         <v>32</v>
       </c>
       <c r="F118">
@@ -2972,7 +2972,7 @@
       <c r="C119" s="3">
         <v>388016</v>
       </c>
-      <c r="E119" s="15">
+      <c r="E119" s="12">
         <v>32</v>
       </c>
       <c r="F119">
@@ -2992,7 +2992,7 @@
       <c r="C120" s="3">
         <v>385028</v>
       </c>
-      <c r="E120" s="15">
+      <c r="E120" s="12">
         <v>32</v>
       </c>
       <c r="F120">
@@ -3012,7 +3012,7 @@
       <c r="C121" s="3">
         <v>225017</v>
       </c>
-      <c r="E121" s="15">
+      <c r="E121" s="12">
         <v>32</v>
       </c>
       <c r="F121">
@@ -3032,7 +3032,7 @@
       <c r="C122" s="3">
         <v>113044</v>
       </c>
-      <c r="E122" s="15">
+      <c r="E122" s="12">
         <v>32</v>
       </c>
       <c r="F122">
@@ -3052,7 +3052,7 @@
       <c r="C123" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E123" s="15">
+      <c r="E123" s="12">
         <v>32</v>
       </c>
       <c r="F123">
@@ -3072,7 +3072,7 @@
       <c r="C124" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E124" s="15">
+      <c r="E124" s="12">
         <v>32</v>
       </c>
       <c r="F124">
@@ -3092,7 +3092,7 @@
       <c r="C125" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E125" s="15">
+      <c r="E125" s="12">
         <v>32</v>
       </c>
       <c r="F125">
@@ -3106,7 +3106,7 @@
       <c r="C126" t="s">
         <v>19</v>
       </c>
-      <c r="E126" s="15">
+      <c r="E126" s="12">
         <v>64</v>
       </c>
       <c r="F126">
@@ -3120,7 +3120,7 @@
       <c r="C127">
         <v>2960592</v>
       </c>
-      <c r="E127" s="15">
+      <c r="E127" s="12">
         <v>64</v>
       </c>
       <c r="F127">
@@ -3134,7 +3134,7 @@
       <c r="C128" t="s">
         <v>26</v>
       </c>
-      <c r="E128" s="15">
+      <c r="E128" s="12">
         <v>64</v>
       </c>
       <c r="F128">
@@ -3148,7 +3148,7 @@
       <c r="C129">
         <v>135069</v>
       </c>
-      <c r="E129" s="15">
+      <c r="E129" s="12">
         <v>64</v>
       </c>
       <c r="F129">
@@ -3162,7 +3162,7 @@
       <c r="C130" t="s">
         <v>18</v>
       </c>
-      <c r="E130" s="15">
+      <c r="E130" s="12">
         <v>64</v>
       </c>
       <c r="F130">
@@ -3176,7 +3176,7 @@
       <c r="C131" t="s">
         <v>8</v>
       </c>
-      <c r="E131" s="15">
+      <c r="E131" s="12">
         <v>64</v>
       </c>
       <c r="F131">

</xml_diff>